<commit_message>
Update DR# 703 USSC (Javelin DNA Pro Printers)_11_26_2021.xlsx
</commit_message>
<xml_diff>
--- a/DR# 703 USSC (Javelin DNA Pro Printers)_11_26_2021.xlsx
+++ b/DR# 703 USSC (Javelin DNA Pro Printers)_11_26_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UBIVELOX\Dropbox\PC\Documents\GitHub\Delivery-Receipt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C2D9226-1A06-427D-A75D-916B0088E75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6063CCF6-CDB7-435D-9165-7AABD7551C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
   <si>
     <t>DELIVERY RECEIPT</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>DR No. 000703</t>
+  </si>
+  <si>
+    <t>Ribbons</t>
+  </si>
+  <si>
+    <t>Black Mono</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1265,7 @@
   <dimension ref="A2:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1381,11 +1387,21 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="10"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="22"/>
+      <c r="A16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="5">
+        <v>2</v>
+      </c>
+      <c r="D16" s="5">
+        <v>2</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="10"/>

</xml_diff>